<commit_message>
230822 iPhoneXS, iPhone SE(2세대), iPhone 11, iPhone 11 Pro Max 추가
</commit_message>
<xml_diff>
--- a/Docs/PhoneSpec 테이블목록.xlsx
+++ b/Docs/PhoneSpec 테이블목록.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdk20\Desktop\new folder\hdk\PhoneSpec\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13AE3AF-B364-45C0-AFEE-9EBE9A8B2A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EE1679-9AC9-4002-BF07-FB8A5DC9B8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADABA816-862A-4067-A46E-B0A232065B46}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="192">
   <si>
     <t>시스템</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -825,14 +825,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"A12 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 4코어 GPU | 8코어 Neural Engine",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"TrueDepth 전면 카메라 | 7MP 사진 | ƒ/2.2 조리개 | Retina Flash | 사진을 위한 스마트 HDR | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 시네마틱 동영상 흔들림 보정(1080p 및 720p)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>"공간 음향 재생 | Dolby Atmos 지원",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -845,35 +837,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"A2101",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"iPhoneXS MAX",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Super Retina HD 디스플레이 | 16.4cm(대각선) 전면 화면 OLED 디스플레이 | HDR 디스플레이 | 2688 x 1242 픽셀 해상도(458ppi) | 1,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 3D Touch | 625 니트 전체 최대 밝기(일반)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"세로 157.5mm | 가로 77.4mm | 두께 7.7mm",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"208g",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 2m, 최대 30분)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"듀얼 12MP 카메라(메인, 망원) | 메인: ƒ/1.8 조리개 | 망원: ƒ/2.4 조리개 | 듀얼 광학 이미지 흔들림 보정(OIS) |  1배, 2배 광학 줌 옵션 | 슬로 싱크 기능을 갖춘 True Tone 플래시 | 사진을 위한 스마트 HDR | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | 동영상을 위한 광학 이미지 흔들림 보정(OIS) | 2배 광학 줌인 | 최대 6배 디지털 줌 | 스테레오 녹음",</t>
+    <t>최초작성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A13 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 4코어 GPU | 8코어 Neural Engine",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"TrueDepth 전면 카메라 | 12MP 사진 | ƒ/2.2 조리개 | Retina Flash | 사진을 위한 스마트 HDR 2 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 프레임) | QuickTake 동영상 | 시네마틱 동영상 흔들림 보정(4K, 1080p 및 720p)",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -899,12 +871,44 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Fi 5 | Bluetooth 5.0 | GPS/GNSS | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
+      <t>Fi 6 | Bluetooth 5.0 | 주변 인식 기능 구현용 초광대역 칩 | GPS/GNSS | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"동영상 재생 : 최대 15시간 | 오디오 재생 : 최대 65시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전(어댑터 별매)",</t>
+    <t>"iPhone 11 Pro Max",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A2218",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Super Retina XDR 디스플레이 | 16.4cm(대각선) 전면 화면 OLED 디스플레이 | HDR 디스플레이 | 2688 x 1242 픽셀 해상도(458ppi) | 2,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 햅틱 터치 | 800 니트 전체 최대 밝기(일반) | 1200 니트 부분 최대 밝기(HDR)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"세로 158.0mm | 가로 77.8mm | 두께 8.1mm",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"226g",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 4m, 최대 30분)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"트리플 12MP 카메라(메인, 울트라 와이드, 망원) | 메인: ƒ/1.8 조리개 | 울트라 와이드: ƒ/2.4 조리개 | 망원: ƒ/2.0 조리개 | 듀얼 광학 이미지 흔들림 보정(OIS) |  0.5배, 1배, 2배 광학 줌 옵션 | 슬로 싱크 기능을 갖춘 True Tone 플래시 | Deep Fusion | 사진을 위한 스마트 HDR 2 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 야간 모드",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | QuickTake 동영상 | 동영상을 위한 광학 이미지 흔들림 보정(OIS) | 2배 광학 줌인, 2배 광학 줌아웃 | 최대 6배 디지털 줌 | 오디오 줌 | 스테레오 녹음",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"동영상 재생 : 최대 20시간 | 동영상 재생(스트리밍) : 최대 12시간 | 오디오 재생 : 최대 80시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전 18W 어댑터 기본 제공",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1172,6 +1176,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1195,9 +1202,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1518,7 +1522,7 @@
   <dimension ref="A3:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1527,11 +1531,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="8" t="s">
         <v>129</v>
       </c>
@@ -1545,13 +1549,13 @@
       <c r="B5" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="13" t="s">
         <v>128</v>
       </c>
@@ -1563,11 +1567,13 @@
       <c r="B6" s="15">
         <v>45151</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
+      <c r="C6" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
       <c r="H6" s="8" t="s">
         <v>131</v>
       </c>
@@ -1598,12 +1604,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1704,9 +1710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651C660F-AA0E-4523-99CB-BC9D04DF4074}">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1728,17 +1734,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="28"/>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1792,10 +1798,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>102</v>
       </c>
       <c r="C3" s="6">
@@ -1828,8 +1834,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1861,8 +1867,8 @@
       <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="26"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1892,8 +1898,8 @@
       <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1923,10 +1929,10 @@
       <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="26" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="6">
@@ -1961,8 +1967,8 @@
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="6">
         <v>2</v>
       </c>
@@ -1994,8 +2000,8 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="6">
         <v>3</v>
       </c>
@@ -2025,8 +2031,8 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="6">
         <v>4</v>
       </c>
@@ -2055,8 +2061,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="6">
         <v>5</v>
       </c>
@@ -2087,10 +2093,10 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="6">
@@ -2123,8 +2129,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="6">
         <v>2</v>
       </c>
@@ -2154,8 +2160,8 @@
       <c r="Q13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="6">
         <v>2</v>
       </c>
@@ -2186,8 +2192,8 @@
       <c r="S14" s="18"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="6">
         <v>3</v>
       </c>
@@ -2220,8 +2226,8 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="6">
         <v>4</v>
       </c>
@@ -2254,8 +2260,8 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="6">
         <v>5</v>
       </c>
@@ -2286,10 +2292,10 @@
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="26" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="6">
@@ -2320,8 +2326,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
       <c r="C19" s="6">
         <v>2</v>
       </c>
@@ -2350,8 +2356,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
       <c r="C20" s="6">
         <v>3</v>
       </c>
@@ -2380,10 +2386,10 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="6">
@@ -2414,8 +2420,8 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="6">
         <v>2</v>
       </c>
@@ -2443,8 +2449,8 @@
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="6">
         <v>3</v>
       </c>
@@ -2472,8 +2478,8 @@
       <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="6">
         <v>4</v>
       </c>
@@ -2501,8 +2507,8 @@
       <c r="Q24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
-      <c r="B25" s="25"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="6">
         <v>5</v>
       </c>
@@ -2530,8 +2536,8 @@
       <c r="Q25" s="18"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="6">
         <v>6</v>
       </c>
@@ -2559,8 +2565,8 @@
       <c r="Q26" s="18"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
-      <c r="B27" s="25"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="6">
         <v>7</v>
       </c>
@@ -2587,8 +2593,8 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="6">
         <v>8</v>
       </c>
@@ -2615,8 +2621,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
-      <c r="B29" s="25"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="6">
         <v>9</v>
       </c>
@@ -2642,8 +2648,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="6">
         <v>10</v>
       </c>
@@ -2670,8 +2676,8 @@
       <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="6">
         <v>11</v>
       </c>
@@ -2703,8 +2709,8 @@
       <c r="Q31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="6">
         <v>12</v>
       </c>
@@ -2729,12 +2735,12 @@
         <v>69</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="6">
         <v>13</v>
       </c>
@@ -2761,12 +2767,12 @@
         <v>108</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="6">
         <v>14</v>
       </c>
@@ -2791,12 +2797,12 @@
         <v>70</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="33" x14ac:dyDescent="0.3">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="6">
         <v>15</v>
       </c>
@@ -2820,14 +2826,14 @@
       <c r="O35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P35" s="28" t="s">
-        <v>183</v>
+      <c r="P35" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="Q35" s="18"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
       <c r="C36" s="6">
         <v>16</v>
       </c>
@@ -2854,13 +2860,13 @@
         <v>72</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="Q36" s="18"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
       <c r="C37" s="6">
         <v>17</v>
       </c>
@@ -2887,13 +2893,13 @@
         <v>73</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Q37" s="18"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
       <c r="C38" s="6">
         <v>18</v>
       </c>
@@ -2920,13 +2926,13 @@
         <v>74</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="6">
         <v>19</v>
       </c>
@@ -2951,13 +2957,13 @@
         <v>75</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="Q39" s="18"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="6">
         <v>20</v>
       </c>
@@ -2982,13 +2988,13 @@
         <v>76</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q40" s="18"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="6">
         <v>21</v>
       </c>
@@ -3013,13 +3019,13 @@
         <v>77</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="Q41" s="18"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="6">
         <v>22</v>
       </c>
@@ -3044,13 +3050,13 @@
         <v>78</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="Q42" s="18"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="6">
         <v>23</v>
       </c>
@@ -3080,8 +3086,8 @@
       <c r="Q43" s="18"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
       <c r="C44" s="6">
         <v>24</v>
       </c>
@@ -3111,8 +3117,8 @@
       <c r="Q44" s="18"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
       <c r="C45" s="6">
         <v>25</v>
       </c>
@@ -3137,13 +3143,13 @@
         <v>84</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="Q45" s="18"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
       <c r="C46" s="6">
         <v>26</v>
       </c>
@@ -3173,8 +3179,8 @@
       <c r="Q46" s="18"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="6">
         <v>27</v>
       </c>
@@ -3204,8 +3210,8 @@
       <c r="Q47" s="18"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="6">
         <v>28</v>
       </c>
@@ -3235,10 +3241,10 @@
       <c r="Q48" s="18"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="26" t="s">
         <v>100</v>
       </c>
       <c r="C49" s="6">
@@ -3272,8 +3278,8 @@
       <c r="Q49" s="18"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="6">
         <v>2</v>
       </c>
@@ -3298,13 +3304,13 @@
         <v>91</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q50" s="18"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="6">
         <v>3</v>
       </c>
@@ -3334,8 +3340,8 @@
       <c r="Q51" s="18"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="6">
         <v>4</v>
       </c>
@@ -3365,8 +3371,8 @@
       <c r="Q52" s="18"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="6">
         <v>5</v>
       </c>
@@ -3396,8 +3402,8 @@
       <c r="Q53" s="18"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="6">
         <v>6</v>
       </c>
@@ -3424,13 +3430,13 @@
         <v>95</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="Q54" s="18"/>
     </row>
     <row r="55" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="6">
         <v>7</v>
       </c>
@@ -3462,8 +3468,8 @@
       <c r="Q55" s="18"/>
     </row>
     <row r="56" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="25"/>
-      <c r="B56" s="25"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="6">
         <v>8</v>
       </c>
@@ -3490,13 +3496,13 @@
         <v>97</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q56" s="18"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="6">
         <v>9</v>
       </c>
@@ -3526,8 +3532,8 @@
       <c r="Q57" s="18"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="6">
         <v>10</v>
       </c>
@@ -3554,8 +3560,8 @@
       <c r="Q58" s="18"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="6">
         <v>11</v>
       </c>
@@ -3579,8 +3585,8 @@
       <c r="Q59" s="18"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="6">
         <v>12</v>
       </c>
@@ -3604,8 +3610,8 @@
       <c r="Q60" s="18"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="25"/>
-      <c r="B61" s="25"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="6">
         <v>13</v>
       </c>
@@ -3630,8 +3636,8 @@
       <c r="Q61" s="18"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
       <c r="C62" s="6">
         <v>14</v>
       </c>
@@ -3656,8 +3662,8 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="6">
         <v>15</v>
       </c>
@@ -3681,8 +3687,8 @@
       <c r="P63" s="3"/>
     </row>
     <row r="64" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="6">
         <v>16</v>
       </c>
@@ -3708,8 +3714,8 @@
       <c r="P64" s="3"/>
     </row>
     <row r="65" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A65" s="25"/>
-      <c r="B65" s="25"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="6">
         <v>17</v>
       </c>
@@ -3736,8 +3742,8 @@
       <c r="Q65" s="18"/>
     </row>
     <row r="66" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A66" s="25"/>
-      <c r="B66" s="25"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="6">
         <v>18</v>
       </c>
@@ -3764,8 +3770,8 @@
       <c r="Q66" s="18"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="25"/>
-      <c r="B67" s="25"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="6">
         <v>19</v>
       </c>
@@ -3792,8 +3798,8 @@
       <c r="Q67" s="18"/>
     </row>
     <row r="68" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="6">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
230825 iPhone11 Pro, iPhone12, iPhone12 mini, iPhone12 Pro Max, iPhone12 Pro, iPhone13 DB 인서트
</commit_message>
<xml_diff>
--- a/Docs/PhoneSpec 테이블목록.xlsx
+++ b/Docs/PhoneSpec 테이블목록.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdk20\Desktop\new folder\hdk\PhoneSpec\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EE1679-9AC9-4002-BF07-FB8A5DC9B8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE55C579-282A-45AB-870B-5F22CE734922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADABA816-862A-4067-A46E-B0A232065B46}"/>
   </bookViews>
@@ -740,7 +740,54 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"충전식 리튬 이온 배터리 내장 | Qi 무선 충전 기능 | 컴퓨터 USB 포트 연결 또는 전원 어댑터로 충전",</t>
+    <t>"음성으로 메시지 전송 | 미리 알림 설정 등 다양한 기능 실행 가능 | 'Siri야'라고 불러 음성만으로 핸즈프리 활성화 | 즐겨 쓰는 앱에서 음성으로 단축어 실행",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Face ID | 얼굴 인식용 TrueDepth 전면 카메라를 통해 지원",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Dolby Vision, HDR10, HLG를 지원하는 HDR",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"공간 음향 재생 | Dolby Atmos 지원",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>최초작성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 6m, 최대 30분)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"GSM/EDGE | UMTS/HSPA+ | DC-HSDPA | CDMA EV-DO Rev. A(일부 모델) | 4x4 MIMO 방식을 지원하는 5G(sub-6 GHz) | Gigabit급 LTE | Wi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>‑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fi 6 | Bluetooth 5.0 | 주변 인식 기능 구현용 초광대역 칩 | GPS, GLONASS, Galileo, QZSS, BeiDou | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
+    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -766,7 +813,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Fi 네트워크) | Wi</t>
+      <t>Fi 네트워크) | 5G 또는 Wi</t>
     </r>
     <r>
       <rPr>
@@ -813,102 +860,55 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"음성으로 메시지 전송 | 미리 알림 설정 등 다양한 기능 실행 가능 | 'Siri야'라고 불러 음성만으로 핸즈프리 활성화 | 즐겨 쓰는 앱에서 음성으로 단축어 실행",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Face ID | 얼굴 인식용 TrueDepth 전면 카메라를 통해 지원",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Dolby Vision, HDR10, HLG를 지원하는 HDR",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"공간 음향 재생 | Dolby Atmos 지원",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"듀얼 SIM(nano-SIM 및 eSIM) | 기존 micro-SIM 카드와 호환되지 않음",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"64GB | 256GB | 512GB",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최초작성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"A13 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 4코어 GPU | 8코어 Neural Engine",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"TrueDepth 전면 카메라 | 12MP 사진 | ƒ/2.2 조리개 | Retina Flash | 사진을 위한 스마트 HDR 2 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 프레임) | QuickTake 동영상 | 시네마틱 동영상 흔들림 보정(4K, 1080p 및 720p)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"GSM/EDGE | UMTS/HSPA+ | DC-HSDPA | CDMA EV-DO Rev. A(일부 모델) | Gigabit급 LTE | Wi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>‑</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fi 6 | Bluetooth 5.0 | 주변 인식 기능 구현용 초광대역 칩 | GPS/GNSS | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"iPhone 11 Pro Max",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"A2218",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Super Retina XDR 디스플레이 | 16.4cm(대각선) 전면 화면 OLED 디스플레이 | HDR 디스플레이 | 2688 x 1242 픽셀 해상도(458ppi) | 2,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 햅틱 터치 | 800 니트 전체 최대 밝기(일반) | 1200 니트 부분 최대 밝기(HDR)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"세로 158.0mm | 가로 77.8mm | 두께 8.1mm",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"226g",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 4m, 최대 30분)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"트리플 12MP 카메라(메인, 울트라 와이드, 망원) | 메인: ƒ/1.8 조리개 | 울트라 와이드: ƒ/2.4 조리개 | 망원: ƒ/2.0 조리개 | 듀얼 광학 이미지 흔들림 보정(OIS) |  0.5배, 1배, 2배 광학 줌 옵션 | 슬로 싱크 기능을 갖춘 True Tone 플래시 | Deep Fusion | 사진을 위한 스마트 HDR 2 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 야간 모드",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | QuickTake 동영상 | 동영상을 위한 광학 이미지 흔들림 보정(OIS) | 2배 광학 줌인, 2배 광학 줌아웃 | 최대 6배 디지털 줌 | 오디오 줌 | 스테레오 녹음",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"동영상 재생 : 최대 20시간 | 동영상 재생(스트리밍) : 최대 12시간 | 오디오 재생 : 최대 80시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전 18W 어댑터 기본 제공",</t>
+    <t>"충전식 리튬 이온 배터리 내장 | MagSafe 및 Qi 무선 충전 기능 | 컴퓨터 USB 포트 연결 또는 전원 어댑터로 충전",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"128GB | 256GB | 512GB",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Super Retina XDR 디스플레이 | 15.4cm(대각선) 전면 화면 OLED 디스플레이 | HDR 디스플레이 | 2532 x 1170 픽셀 해상도(460ppi) | 2,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 햅틱 터치 | 800 니트 전체 최대 밝기(일반) | 1200 니트 부분 최대 밝기(HDR)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"iPhone 13",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A2633",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"세로 146.7mm | 가로 71.5mm | 두께 7.65mm",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"173g",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A15 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 4코어 GPU | 16코어 Neural Engine",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"듀얼 12MP 카메라 시스템(메인, 울트라 와이드) | 메인: ƒ/1.6 조리개 | 울트라 와이드: ƒ/2.4 조리개 | 센서 시프트 광학 이미지 흔들림 보정(OIS) |  0.5배, 1배 광학 줌 옵션 | 슬로 싱크 기능을 갖춘 True Tone 플래시 | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 야간 모드 | 사진 스타일",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 얕은 피사계 심도 효과로 동영상을 촬영하는 시네마틱 모드(1080p 동영상, 초당 30 프레임) | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | 야간 모드 타임랩스 | QuickTake 동영상 | 동영상을 위한 광학 이미지 흔들림 보정(OIS) | 2배 광학 줌아웃 | 최대 3배 디지털 줌 | 오디오 줌 | 스테레오 녹음",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"TrueDepth 전면 카메라 | 12MP 사진 | ƒ/2.2 조리개 | Retina Flash | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 야간 모드 | 사진 스타일 | 4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 시네마틱 모드(1080p 동영상, 초당 30 프레임) | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 30 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 프레임) | QuickTake 동영상 | 시네마틱 동영상 흔들림 보정(4K, 1080p 및 720p)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"동영상 재생 : 최대 19시간 | 동영상 재생(스트리밍) : 최대 15시간 | 오디오 재생 : 최대 75시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전(어댑터 별매)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"듀얼 SIM(nano-SIM 및 eSIM) | 듀얼 eSIM 지원 | 기존 micro-SIM 카드와 호환되지 않음",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1194,14 +1194,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1568,7 +1568,7 @@
         <v>45151</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -1711,8 +1711,8 @@
   <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P40" sqref="P40"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1734,17 +1734,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="28"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1798,10 +1798,10 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>102</v>
       </c>
       <c r="C3" s="6">
@@ -1834,8 +1834,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1867,8 +1867,8 @@
       <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1898,8 +1898,8 @@
       <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1929,10 +1929,10 @@
       <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="6">
@@ -1967,8 +1967,8 @@
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="6">
         <v>2</v>
       </c>
@@ -2000,8 +2000,8 @@
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="6">
         <v>3</v>
       </c>
@@ -2031,8 +2031,8 @@
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="6">
         <v>4</v>
       </c>
@@ -2061,8 +2061,8 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="6">
         <v>5</v>
       </c>
@@ -2093,10 +2093,10 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="6">
@@ -2129,8 +2129,8 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="6">
         <v>2</v>
       </c>
@@ -2160,8 +2160,8 @@
       <c r="Q13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="6">
         <v>2</v>
       </c>
@@ -2192,8 +2192,8 @@
       <c r="S14" s="18"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="6">
         <v>3</v>
       </c>
@@ -2226,8 +2226,8 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="6">
         <v>4</v>
       </c>
@@ -2260,8 +2260,8 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="6">
         <v>5</v>
       </c>
@@ -2292,10 +2292,10 @@
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="28" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="6">
@@ -2326,8 +2326,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="6">
         <v>2</v>
       </c>
@@ -2356,8 +2356,8 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="6">
         <v>3</v>
       </c>
@@ -2386,10 +2386,10 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="6">
@@ -2420,8 +2420,8 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="6">
         <v>2</v>
       </c>
@@ -2449,8 +2449,8 @@
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="6">
         <v>3</v>
       </c>
@@ -2478,8 +2478,8 @@
       <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="6">
         <v>4</v>
       </c>
@@ -2507,8 +2507,8 @@
       <c r="Q24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="6">
         <v>5</v>
       </c>
@@ -2536,8 +2536,8 @@
       <c r="Q25" s="18"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="6">
         <v>6</v>
       </c>
@@ -2565,8 +2565,8 @@
       <c r="Q26" s="18"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="6">
         <v>7</v>
       </c>
@@ -2593,8 +2593,8 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="6">
         <v>8</v>
       </c>
@@ -2621,8 +2621,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="6">
         <v>9</v>
       </c>
@@ -2648,8 +2648,8 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="6">
         <v>10</v>
       </c>
@@ -2676,8 +2676,8 @@
       <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="6">
         <v>11</v>
       </c>
@@ -2709,8 +2709,8 @@
       <c r="Q31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="6">
         <v>12</v>
       </c>
@@ -2735,12 +2735,12 @@
         <v>69</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="6">
         <v>13</v>
       </c>
@@ -2767,12 +2767,12 @@
         <v>108</v>
       </c>
       <c r="P33" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="6">
         <v>14</v>
       </c>
@@ -2797,12 +2797,12 @@
         <v>70</v>
       </c>
       <c r="P34" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="6">
         <v>15</v>
       </c>
@@ -2827,13 +2827,13 @@
         <v>71</v>
       </c>
       <c r="P35" s="20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Q35" s="18"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="6">
         <v>16</v>
       </c>
@@ -2860,13 +2860,13 @@
         <v>72</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q36" s="18"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="6">
         <v>17</v>
       </c>
@@ -2893,13 +2893,13 @@
         <v>73</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="Q37" s="18"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="6">
         <v>18</v>
       </c>
@@ -2926,13 +2926,13 @@
         <v>74</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="6">
         <v>19</v>
       </c>
@@ -2957,13 +2957,13 @@
         <v>75</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="Q39" s="18"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="6">
         <v>20</v>
       </c>
@@ -2988,13 +2988,13 @@
         <v>76</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Q40" s="18"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="6">
         <v>21</v>
       </c>
@@ -3019,13 +3019,13 @@
         <v>77</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="Q41" s="18"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="6">
         <v>22</v>
       </c>
@@ -3050,13 +3050,13 @@
         <v>78</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="Q42" s="18"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="6">
         <v>23</v>
       </c>
@@ -3086,8 +3086,8 @@
       <c r="Q43" s="18"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="6">
         <v>24</v>
       </c>
@@ -3117,8 +3117,8 @@
       <c r="Q44" s="18"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="6">
         <v>25</v>
       </c>
@@ -3143,13 +3143,13 @@
         <v>84</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="Q45" s="18"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="6">
         <v>26</v>
       </c>
@@ -3174,13 +3174,13 @@
         <v>85</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="Q46" s="18"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="6">
         <v>27</v>
       </c>
@@ -3210,8 +3210,8 @@
       <c r="Q47" s="18"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="6">
         <v>28</v>
       </c>
@@ -3236,15 +3236,15 @@
         <v>89</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="Q48" s="18"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="28" t="s">
         <v>100</v>
       </c>
       <c r="C49" s="6">
@@ -3278,8 +3278,8 @@
       <c r="Q49" s="18"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="6">
         <v>2</v>
       </c>
@@ -3304,13 +3304,13 @@
         <v>91</v>
       </c>
       <c r="P50" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q50" s="18"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="6">
         <v>3</v>
       </c>
@@ -3335,13 +3335,13 @@
         <v>92</v>
       </c>
       <c r="P51" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q51" s="18"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="6">
         <v>4</v>
       </c>
@@ -3366,13 +3366,13 @@
         <v>93</v>
       </c>
       <c r="P52" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q52" s="18"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="6">
         <v>5</v>
       </c>
@@ -3397,13 +3397,13 @@
         <v>94</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="Q53" s="18"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="6">
         <v>6</v>
       </c>
@@ -3430,13 +3430,13 @@
         <v>95</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q54" s="18"/>
     </row>
     <row r="55" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="6">
         <v>7</v>
       </c>
@@ -3468,8 +3468,8 @@
       <c r="Q55" s="18"/>
     </row>
     <row r="56" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="6">
         <v>8</v>
       </c>
@@ -3496,13 +3496,13 @@
         <v>97</v>
       </c>
       <c r="P56" s="3" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="Q56" s="18"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="6">
         <v>9</v>
       </c>
@@ -3532,8 +3532,8 @@
       <c r="Q57" s="18"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="6">
         <v>10</v>
       </c>
@@ -3560,8 +3560,8 @@
       <c r="Q58" s="18"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="6">
         <v>11</v>
       </c>
@@ -3585,8 +3585,8 @@
       <c r="Q59" s="18"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="6">
         <v>12</v>
       </c>
@@ -3610,8 +3610,8 @@
       <c r="Q60" s="18"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="6">
         <v>13</v>
       </c>
@@ -3636,8 +3636,8 @@
       <c r="Q61" s="18"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="6">
         <v>14</v>
       </c>
@@ -3662,8 +3662,8 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="6">
         <v>15</v>
       </c>
@@ -3687,8 +3687,8 @@
       <c r="P63" s="3"/>
     </row>
     <row r="64" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="6">
         <v>16</v>
       </c>
@@ -3714,8 +3714,8 @@
       <c r="P64" s="3"/>
     </row>
     <row r="65" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
+      <c r="A65" s="28"/>
+      <c r="B65" s="28"/>
       <c r="C65" s="6">
         <v>17</v>
       </c>
@@ -3742,8 +3742,8 @@
       <c r="Q65" s="18"/>
     </row>
     <row r="66" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
+      <c r="A66" s="28"/>
+      <c r="B66" s="28"/>
       <c r="C66" s="6">
         <v>18</v>
       </c>
@@ -3770,8 +3770,8 @@
       <c r="Q66" s="18"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="28"/>
       <c r="C67" s="6">
         <v>19</v>
       </c>
@@ -3798,8 +3798,8 @@
       <c r="Q67" s="18"/>
     </row>
     <row r="68" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="6">
         <v>20</v>
       </c>
@@ -3871,12 +3871,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A7:A11"/>
     <mergeCell ref="A49:A68"/>
     <mergeCell ref="B49:B68"/>
     <mergeCell ref="A21:A48"/>
@@ -3885,6 +3879,12 @@
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
230827 iPhone 14, iPhone 14 Plus, iPhone 14 Pro, iPhone 14 Pro Max data insert
</commit_message>
<xml_diff>
--- a/Docs/PhoneSpec 테이블목록.xlsx
+++ b/Docs/PhoneSpec 테이블목록.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdk20\Desktop\new folder\hdk\PhoneSpec\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E333471C-CD7F-4771-BB88-DBBD6DB88C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366BDE23-E351-49B8-95C2-6E7E30378007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{ADABA816-862A-4067-A46E-B0A232065B46}"/>
   </bookViews>
@@ -689,10 +689,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"긴급 구조 요청",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>"매장, 앱, 웹사이트에서 Touch ID를 이용해 iPhone으로 결제",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -706,10 +702,6 @@
   </si>
   <si>
     <t>"KT | LGU+ | SKT",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">"3축 자이로 | 가속도계 | 근접 센서 | 주변광 센서 | 기압계", </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -744,50 +736,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>최초작성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 6m, 최대 30분)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"긴급 구조 요청 | 충돌 감지",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>"Face ID | 얼굴 인식용 TrueDepth 전면 카메라를 통해 지원",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Dolby Vision, HDR10, HLG를 지원하는 HDR",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"공간 음향 재생 | Dolby Atmos 지원",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>최초작성</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"IEC 규격 60529하의 IP68 등급 획득(최대 수심 6m, 최대 30분)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>"GSM/EDGE | UMTS/HSPA+ | DC-HSDPA | CDMA EV-DO Rev. A(일부 모델) | 4x4 MIMO 방식을 지원하는 5G(sub-6 GHz) | Gigabit급 LTE | Wi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>‑</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fi 6 | Bluetooth 5.0 | 주변 인식 기능 구현용 초광대역 칩 | GPS, GLONASS, Galileo, QZSS, BeiDou | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -860,55 +821,94 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>"공간 음향 재생 | Dolby Atmos 지원",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Dolby Vision, HDR10, HLG를 지원하는 HDR",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>"충전식 리튬 이온 배터리 내장 | MagSafe 및 Qi 무선 충전 기능 | 컴퓨터 USB 포트 연결 또는 전원 어댑터로 충전",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>"128GB | 256GB | 512GB",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Super Retina XDR 디스플레이 | 15.4cm(대각선) 전면 화면 OLED 디스플레이 | HDR 디스플레이 | 2532 x 1170 픽셀 해상도(460ppi) | 2,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 햅틱 터치 | 800 니트 전체 최대 밝기(일반) | 1200 니트 부분 최대 밝기(HDR)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"iPhone 13",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"A2633",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"세로 146.7mm | 가로 71.5mm | 두께 7.65mm",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"173g",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"A15 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 4코어 GPU | 16코어 Neural Engine",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"듀얼 12MP 카메라 시스템(메인, 울트라 와이드) | 메인: ƒ/1.6 조리개 | 울트라 와이드: ƒ/2.4 조리개 | 센서 시프트 광학 이미지 흔들림 보정(OIS) |  0.5배, 1배 광학 줌 옵션 | 슬로 싱크 기능을 갖춘 True Tone 플래시 | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 야간 모드 | 사진 스타일",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 얕은 피사계 심도 효과로 동영상을 촬영하는 시네마틱 모드(1080p 동영상, 초당 30 프레임) | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 60 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | 야간 모드 타임랩스 | QuickTake 동영상 | 동영상을 위한 광학 이미지 흔들림 보정(OIS) | 2배 광학 줌아웃 | 최대 3배 디지털 줌 | 오디오 줌 | 스테레오 녹음",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"TrueDepth 전면 카메라 | 12MP 사진 | ƒ/2.2 조리개 | Retina Flash | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 야간 모드 | 사진 스타일 | 4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 시네마틱 모드(1080p 동영상, 초당 30 프레임) | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 30 프레임) | 1080p 슬로 모션 동영상 지원(초당 120 프레임) | QuickTake 동영상 | 시네마틱 동영상 흔들림 보정(4K, 1080p 및 720p)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"동영상 재생 : 최대 19시간 | 동영상 재생(스트리밍) : 최대 15시간 | 오디오 재생 : 최대 75시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전(어댑터 별매)",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"듀얼 SIM(nano-SIM 및 eSIM) | 듀얼 eSIM 지원 | 기존 micro-SIM 카드와 호환되지 않음",</t>
+    <t>"듀얼 SIM(2개의 활성 eSIM 또는 nano-SIM 및 eSIM) | 듀얼 eSIM 지원",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"128GB | 256GB | 512GB | 1TB",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A16 Bionic 칩 | 6코어 CPU(성능 코어 2개 및 효율 코어 4개) | 5코어 GPU | 16코어 Neural Engine",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"프로급 카메라 시스템(48MP 메인, 12MP 울트라 와이드, 12MP 망원) | 메인: ƒ/1.78 조리개 | 울트라 와이드: ƒ/2.2 조리개 | 망원: ƒ/2.8 조리개 | 2세대 센서 시프트 광학 이미지 흔들림 보정(OIS) | 0.5배, 1배, 2배, 3배 광학 줌 옵션 | 적응형 True Tone 플래시 | Photonic Engine | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 야간 모드 | 야간 모드 인물 사진 | 사진 스타일 접사 사진 | Apple ProRAW",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 얕은 피사계 심도 효과로 동영상을 촬영하는 시네마틱 모드(4K HDR, 초당 최대 30 프레임) | 액션 모드 | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 60 프레임) | 최대 4K ProRes 동영상 촬영(초당 30 프레임)(128GB 모델은 초당 30 프레임의 1080p 동영상) | 접사 동영상 촬영(슬로 모션 및 타임랩스 포함) | 1080p 슬로 모션 동영상 지원(초당 120 또는 240 프레임) | 타임랩스 동영상(동영상 흔들림 보정 포함) | 야간 모드 타임랩스 | QuickTake 동영상 | 동영상을 위한 센서 시프트 광학 이미지 흔들림 보정(OIS) | 3배 광학 줌인, 2배 광학 줌아웃 | 최대 9배 디지털 줌 | 오디오 줌 | 스테레오 녹음",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"TrueDepth 전면 카메라 | 12MP 사진 | ƒ/1.9 조리개 | Retina Flash | Photonic Engine | Deep Fusion | 사진을 위한 스마트 HDR 4 | 향상된 보케 효과 및 심도 제어 기능을 지원하는 인물 사진 모드 | 6가지 효과의 인물 사진 조명(자연 조명, 스튜디오 조명, 윤곽 조명, 무대 조명, 무대 조명 모노, 하이키 모노) | 애니모티콘과 미모티콘 | 야간 모드 | 사진 스타일 | 4K 동영상 촬영(초당 24, 25, 30 또는 60 프레임) | 1080p HD 동영상 촬영(초당 25, 30 또는 60 프레임) | 최대 4K HDR 시네마틱 모드 동영상 촬영(초당 30 프레임) | Dolby Vision 방식으로 최대 4K HDR 동영상 촬영(초당 60 프레임) | 최대 4K ProRes 동영상 촬영(초당 30 프레임)(128GB 모델은 초당 30 프레임의 1080p 동영상) | 1080p 슬로 모션 동영상 지원(초당 120 프레임) | QuickTake 동영상 | 시네마틱 동영상 흔들림 보정(4K, 1080p 및 720p)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>"GSM/EDGE | UMTS/HSPA+ | DC-HSDPA | 4x4 MIMO 방식을 지원하는 5G(sub-6 GHz) | Gigabit LTE | Wi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>‑</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fi 6 | Bluetooth 5.3 | 주변 인식 기능 구현용 초광대역 칩 | 정밀 이중 주파수 GPS(GPS, GLONASS, Galileo, QZSS, BeiDou) | LTE 음성 통화(VoLTE) | 리더 모드를 지원하는 NFC | 예비 전력으로 작동하는 익스프레스 카드 기능" ,</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">"LiDAR 스캐너 | 하이 다이내믹 레인지 자이로 | 고중력 가속도계 | 근접 센서 | 듀얼 주변광 센서 | 기압계", </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"iPhone 14 Pro",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"A2890",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Super Retina XDR 디스플레이 | 15.5cm(대각선) 전면 화면 OLED 디스플레이 | Dynamic Island | 최대 120Hz 가변 재생률을 제공하는 ProMotion 기술 | 상시표시형 디스플레이 | HDR 디스플레이 | 2556 x 1179 픽셀 해상도(460ppi) | 2,000,000:1 명암비(일반) | True Tone 디스플레이 | 와이드 컬러 디스플레이(P3) | 햅틱 터치 | 1000 니트 전체 최대 밝기(일반) | 1600 니트 부분 최대 밝기(HDR) | 2000 니트 부분 최대 밝기(야외)",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"세로 147.5mm | 가로 71.5mm | 두께 7.85mm",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"206g",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"동영상 재생 : 최대 23시간 | 동영상 재생(스트리밍) : 최대 20시간 | 오디오 재생 : 최대 75시간 | 급속 충전 가능 20W 이상 규격의 어댑터 사용 시 30분에 최대 50% 충전(어댑터 별매)",</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1115,7 +1115,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1173,11 +1173,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1531,11 +1534,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="8" t="s">
         <v>129</v>
       </c>
@@ -1549,13 +1552,13 @@
       <c r="B5" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="13" t="s">
         <v>128</v>
       </c>
@@ -1567,13 +1570,13 @@
       <c r="B6" s="15">
         <v>45151</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
+      <c r="C6" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="8" t="s">
         <v>131</v>
       </c>
@@ -1604,12 +1607,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -1710,9 +1713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{651C660F-AA0E-4523-99CB-BC9D04DF4074}">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P60" sqref="P60"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P37" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1726,7 +1729,7 @@
     <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="215.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="215.375" style="20" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1734,17 +1737,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="28"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1757,8 +1760,8 @@
       <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
-        <v>167</v>
+      <c r="P1" s="20" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1792,16 +1795,16 @@
       <c r="J2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="19" t="str">
+      <c r="P2" s="21" t="str">
         <f t="shared" ref="P2:P27" si="0">""&amp;D22&amp;","</f>
         <v>DEVICE_TYPE,</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>102</v>
       </c>
       <c r="C3" s="6">
@@ -1828,14 +1831,14 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="P3" s="19" t="str">
+      <c r="P3" s="21" t="str">
         <f t="shared" si="0"/>
         <v>PRODUCTNM,</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1860,15 +1863,15 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="P4" s="19" t="str">
+      <c r="P4" s="21" t="str">
         <f t="shared" si="0"/>
         <v>MODELNM,</v>
       </c>
       <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1891,15 +1894,15 @@
       <c r="J5" s="7"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="P5" s="19" t="str">
+      <c r="P5" s="21" t="str">
         <f t="shared" si="0"/>
         <v>STORAGE,</v>
       </c>
       <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1922,17 +1925,17 @@
       <c r="J6" s="7"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="P6" s="19" t="str">
+      <c r="P6" s="21" t="str">
         <f t="shared" si="0"/>
         <v>DISPLAY,</v>
       </c>
       <c r="Q6" s="18"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="6">
@@ -1959,7 +1962,7 @@
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="P7" s="19" t="str">
+      <c r="P7" s="21" t="str">
         <f t="shared" si="0"/>
         <v>SIZE,</v>
       </c>
@@ -1967,8 +1970,8 @@
       <c r="S7" s="18"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="6">
         <v>2</v>
       </c>
@@ -1993,15 +1996,15 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="P8" s="19" t="str">
+      <c r="P8" s="21" t="str">
         <f t="shared" si="0"/>
         <v>WEIGHT,</v>
       </c>
       <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="6">
         <v>3</v>
       </c>
@@ -2024,15 +2027,15 @@
       <c r="J9" s="7"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="P9" s="19" t="str">
+      <c r="P9" s="21" t="str">
         <f t="shared" si="0"/>
         <v>PROOF,</v>
       </c>
       <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="6">
         <v>4</v>
       </c>
@@ -2055,14 +2058,14 @@
       <c r="J10" s="7"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="P10" s="19" t="str">
+      <c r="P10" s="21" t="str">
         <f t="shared" si="0"/>
         <v>CHIP,</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="6">
         <v>5</v>
       </c>
@@ -2087,16 +2090,16 @@
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="P11" s="19" t="str">
+      <c r="P11" s="21" t="str">
         <f t="shared" si="0"/>
         <v>CAMERA,</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="6">
@@ -2123,14 +2126,14 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="P12" s="19" t="str">
+      <c r="P12" s="21" t="str">
         <f t="shared" si="0"/>
         <v>VIDEO,</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="6">
         <v>2</v>
       </c>
@@ -2153,15 +2156,15 @@
       <c r="J13" s="5"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="P13" s="19" t="str">
+      <c r="P13" s="21" t="str">
         <f t="shared" si="0"/>
         <v>F_CAMERA,</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="6">
         <v>2</v>
       </c>
@@ -2184,7 +2187,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="P14" s="19" t="str">
+      <c r="P14" s="21" t="str">
         <f t="shared" si="0"/>
         <v>SAFETY,</v>
       </c>
@@ -2192,8 +2195,8 @@
       <c r="S14" s="18"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="6">
         <v>3</v>
       </c>
@@ -2218,7 +2221,7 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="P15" s="19" t="str">
+      <c r="P15" s="21" t="str">
         <f t="shared" si="0"/>
         <v>AGENCY,</v>
       </c>
@@ -2226,8 +2229,8 @@
       <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="6">
         <v>4</v>
       </c>
@@ -2252,7 +2255,7 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="P16" s="19" t="str">
+      <c r="P16" s="21" t="str">
         <f t="shared" si="0"/>
         <v>CELL_WIRE,</v>
       </c>
@@ -2260,8 +2263,8 @@
       <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="6">
         <v>5</v>
       </c>
@@ -2284,7 +2287,7 @@
       <c r="J17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="P17" s="19" t="str">
+      <c r="P17" s="21" t="str">
         <f t="shared" si="0"/>
         <v>AUTH,</v>
       </c>
@@ -2292,10 +2295,10 @@
       <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="27" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="6">
@@ -2320,14 +2323,14 @@
       <c r="J18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="P18" s="19" t="str">
+      <c r="P18" s="21" t="str">
         <f t="shared" si="0"/>
         <v>PAY,</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="6">
         <v>2</v>
       </c>
@@ -2350,14 +2353,14 @@
       <c r="J19" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="P19" s="19" t="str">
+      <c r="P19" s="21" t="str">
         <f t="shared" si="0"/>
         <v>VIDEOCALL,</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="6">
         <v>3</v>
       </c>
@@ -2380,16 +2383,16 @@
       <c r="J20" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="P20" s="19" t="str">
+      <c r="P20" s="21" t="str">
         <f t="shared" si="0"/>
         <v>VOICECALL,</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="6">
@@ -2414,14 +2417,14 @@
       <c r="J21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="P21" s="19" t="str">
+      <c r="P21" s="21" t="str">
         <f t="shared" si="0"/>
         <v>PLAYAUDIO,</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="6">
         <v>2</v>
       </c>
@@ -2442,15 +2445,15 @@
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
-      <c r="P22" s="19" t="str">
+      <c r="P22" s="21" t="str">
         <f t="shared" si="0"/>
         <v>PLAYVIDEO,</v>
       </c>
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="6">
         <v>3</v>
       </c>
@@ -2471,15 +2474,15 @@
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
-      <c r="P23" s="19" t="str">
+      <c r="P23" s="21" t="str">
         <f t="shared" si="0"/>
         <v>SIRI,</v>
       </c>
       <c r="Q23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="6">
         <v>4</v>
       </c>
@@ -2500,15 +2503,15 @@
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
-      <c r="P24" s="19" t="str">
+      <c r="P24" s="21" t="str">
         <f t="shared" si="0"/>
         <v>POWER,</v>
       </c>
       <c r="Q24" s="18"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="6">
         <v>5</v>
       </c>
@@ -2529,15 +2532,15 @@
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
-      <c r="P25" s="19" t="str">
+      <c r="P25" s="21" t="str">
         <f t="shared" si="0"/>
         <v>BATTERY,</v>
       </c>
       <c r="Q25" s="18"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="6">
         <v>6</v>
       </c>
@@ -2558,15 +2561,15 @@
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
-      <c r="P26" s="19" t="str">
+      <c r="P26" s="21" t="str">
         <f t="shared" si="0"/>
         <v>SENSOR,</v>
       </c>
       <c r="Q26" s="18"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="6">
         <v>7</v>
       </c>
@@ -2587,14 +2590,14 @@
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
-      <c r="P27" s="19" t="str">
+      <c r="P27" s="21" t="str">
         <f t="shared" si="0"/>
         <v>SIM,</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="6">
         <v>8</v>
       </c>
@@ -2615,14 +2618,14 @@
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="P28" s="19" t="str">
+      <c r="P28" s="21" t="str">
         <f>""&amp;D48&amp;""</f>
         <v>CONNECTOR</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="6">
         <v>9</v>
       </c>
@@ -2643,13 +2646,13 @@
       </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
-      <c r="P29" s="3" t="s">
+      <c r="P29" s="19" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="6">
         <v>10</v>
       </c>
@@ -2670,14 +2673,14 @@
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="P30" s="3" t="s">
+      <c r="P30" s="19" t="s">
         <v>162</v>
       </c>
       <c r="Q30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="6">
         <v>11</v>
       </c>
@@ -2703,14 +2706,14 @@
       <c r="O31" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="P31" s="19" t="s">
         <v>163</v>
       </c>
       <c r="Q31" s="18"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="6">
         <v>12</v>
       </c>
@@ -2734,13 +2737,13 @@
       <c r="O32" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="P32" s="3" t="s">
-        <v>182</v>
+      <c r="P32" s="19" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="6">
         <v>13</v>
       </c>
@@ -2766,13 +2769,13 @@
       <c r="O33" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="P33" s="3" t="s">
-        <v>183</v>
+      <c r="P33" s="19" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="6">
         <v>14</v>
       </c>
@@ -2796,13 +2799,13 @@
       <c r="O34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="P34" s="3" t="s">
-        <v>180</v>
+      <c r="P34" s="19" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="6">
         <v>15</v>
       </c>
@@ -2826,14 +2829,14 @@
       <c r="O35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P35" s="20" t="s">
-        <v>181</v>
+      <c r="P35" s="19" t="s">
+        <v>188</v>
       </c>
       <c r="Q35" s="18"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="6">
         <v>16</v>
       </c>
@@ -2859,14 +2862,14 @@
       <c r="O36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="P36" s="3" t="s">
-        <v>184</v>
+      <c r="P36" s="19" t="s">
+        <v>189</v>
       </c>
       <c r="Q36" s="18"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="6">
         <v>17</v>
       </c>
@@ -2892,14 +2895,14 @@
       <c r="O37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="P37" s="3" t="s">
-        <v>185</v>
+      <c r="P37" s="19" t="s">
+        <v>190</v>
       </c>
       <c r="Q37" s="18"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="6">
         <v>18</v>
       </c>
@@ -2925,14 +2928,14 @@
       <c r="O38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="P38" s="3" t="s">
-        <v>176</v>
+      <c r="P38" s="19" t="s">
+        <v>171</v>
       </c>
       <c r="Q38" s="18"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="6">
         <v>19</v>
       </c>
@@ -2956,14 +2959,14 @@
       <c r="O39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="P39" s="3" t="s">
-        <v>186</v>
+      <c r="P39" s="19" t="s">
+        <v>180</v>
       </c>
       <c r="Q39" s="18"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
+    <row r="40" spans="1:17" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="6">
         <v>20</v>
       </c>
@@ -2987,14 +2990,14 @@
       <c r="O40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="P40" s="3" t="s">
-        <v>187</v>
+      <c r="P40" s="19" t="s">
+        <v>181</v>
       </c>
       <c r="Q40" s="18"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
+    <row r="41" spans="1:17" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="6">
         <v>21</v>
       </c>
@@ -3018,14 +3021,14 @@
       <c r="O41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="P41" s="3" t="s">
-        <v>188</v>
+      <c r="P41" s="19" t="s">
+        <v>182</v>
       </c>
       <c r="Q41" s="18"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
+    <row r="42" spans="1:17" ht="66" x14ac:dyDescent="0.3">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="6">
         <v>22</v>
       </c>
@@ -3049,14 +3052,14 @@
       <c r="O42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="P42" s="3" t="s">
-        <v>189</v>
+      <c r="P42" s="19" t="s">
+        <v>183</v>
       </c>
       <c r="Q42" s="18"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="6">
         <v>23</v>
       </c>
@@ -3080,14 +3083,14 @@
       <c r="O43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="P43" s="3" t="s">
-        <v>164</v>
+      <c r="P43" s="19" t="s">
+        <v>172</v>
       </c>
       <c r="Q43" s="18"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="6">
         <v>24</v>
       </c>
@@ -3111,14 +3114,14 @@
       <c r="O44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="P44" s="3" t="s">
-        <v>168</v>
+      <c r="P44" s="19" t="s">
+        <v>167</v>
       </c>
       <c r="Q44" s="18"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
+    <row r="45" spans="1:17" ht="33" x14ac:dyDescent="0.3">
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="6">
         <v>25</v>
       </c>
@@ -3142,14 +3145,14 @@
       <c r="O45" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="P45" s="3" t="s">
-        <v>177</v>
+      <c r="P45" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="Q45" s="18"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="6">
         <v>26</v>
       </c>
@@ -3173,14 +3176,14 @@
       <c r="O46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="P46" s="3" t="s">
-        <v>172</v>
+      <c r="P46" s="19" t="s">
+        <v>173</v>
       </c>
       <c r="Q46" s="18"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="6">
         <v>27</v>
       </c>
@@ -3204,14 +3207,14 @@
       <c r="O47" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="P47" s="3" t="s">
-        <v>165</v>
+      <c r="P47" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="Q47" s="18"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
+    <row r="48" spans="1:17" ht="33" x14ac:dyDescent="0.3">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="6">
         <v>28</v>
       </c>
@@ -3235,16 +3238,16 @@
       <c r="O48" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="P48" s="3" t="s">
-        <v>178</v>
+      <c r="P48" s="19" t="s">
+        <v>174</v>
       </c>
       <c r="Q48" s="18"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="27" t="s">
         <v>100</v>
       </c>
       <c r="C49" s="6">
@@ -3272,14 +3275,14 @@
       <c r="O49" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="P49" s="3" t="s">
-        <v>170</v>
+      <c r="P49" s="19" t="s">
+        <v>168</v>
       </c>
       <c r="Q49" s="18"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="6">
         <v>2</v>
       </c>
@@ -3303,14 +3306,14 @@
       <c r="O50" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="P50" s="3" t="s">
-        <v>174</v>
+      <c r="P50" s="19" t="s">
+        <v>175</v>
       </c>
       <c r="Q50" s="18"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="6">
         <v>3</v>
       </c>
@@ -3334,14 +3337,14 @@
       <c r="O51" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="P51" s="3" t="s">
-        <v>173</v>
+      <c r="P51" s="19" t="s">
+        <v>176</v>
       </c>
       <c r="Q51" s="18"/>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
-      <c r="B52" s="26"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="6">
         <v>4</v>
       </c>
@@ -3365,14 +3368,14 @@
       <c r="O52" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="P52" s="3" t="s">
-        <v>171</v>
+      <c r="P52" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="Q52" s="18"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="6">
         <v>5</v>
       </c>
@@ -3396,14 +3399,14 @@
       <c r="O53" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="P53" s="3" t="s">
-        <v>179</v>
+      <c r="P53" s="19" t="s">
+        <v>177</v>
       </c>
       <c r="Q53" s="18"/>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="6">
         <v>6</v>
       </c>
@@ -3429,14 +3432,14 @@
       <c r="O54" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P54" s="3" t="s">
-        <v>190</v>
+      <c r="P54" s="19" t="s">
+        <v>191</v>
       </c>
       <c r="Q54" s="18"/>
     </row>
     <row r="55" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="6">
         <v>7</v>
       </c>
@@ -3462,14 +3465,14 @@
       <c r="O55" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="P55" s="3" t="s">
-        <v>169</v>
+      <c r="P55" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="Q55" s="18"/>
     </row>
     <row r="56" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="6">
         <v>8</v>
       </c>
@@ -3495,14 +3498,14 @@
       <c r="O56" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="P56" s="3" t="s">
-        <v>191</v>
+      <c r="P56" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="Q56" s="18"/>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="6">
         <v>9</v>
       </c>
@@ -3526,14 +3529,14 @@
       <c r="O57" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="P57" s="3" t="s">
-        <v>166</v>
+      <c r="P57" s="19" t="s">
+        <v>165</v>
       </c>
       <c r="Q57" s="18"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="6">
         <v>10</v>
       </c>
@@ -3554,14 +3557,14 @@
       </c>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
-      <c r="P58" s="3" t="s">
+      <c r="P58" s="19" t="s">
         <v>160</v>
       </c>
       <c r="Q58" s="18"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="6">
         <v>11</v>
       </c>
@@ -3585,8 +3588,8 @@
       <c r="Q59" s="18"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="6">
         <v>12</v>
       </c>
@@ -3610,8 +3613,8 @@
       <c r="Q60" s="18"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
       <c r="C61" s="6">
         <v>13</v>
       </c>
@@ -3632,12 +3635,12 @@
       </c>
       <c r="I61" s="8"/>
       <c r="J61" s="8"/>
-      <c r="P61" s="3"/>
+      <c r="P61" s="19"/>
       <c r="Q61" s="18"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="26"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
       <c r="C62" s="6">
         <v>14</v>
       </c>
@@ -3662,8 +3665,8 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
       <c r="C63" s="6">
         <v>15</v>
       </c>
@@ -3684,11 +3687,11 @@
       </c>
       <c r="I63" s="8"/>
       <c r="J63" s="8"/>
-      <c r="P63" s="3"/>
+      <c r="P63" s="19"/>
     </row>
     <row r="64" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="6">
         <v>16</v>
       </c>
@@ -3711,11 +3714,11 @@
       <c r="J64" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="P64" s="3"/>
+      <c r="P64" s="19"/>
     </row>
     <row r="65" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="6">
         <v>17</v>
       </c>
@@ -3738,12 +3741,12 @@
       <c r="J65" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="P65" s="3"/>
+      <c r="P65" s="19"/>
       <c r="Q65" s="18"/>
     </row>
     <row r="66" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
       <c r="C66" s="6">
         <v>18</v>
       </c>
@@ -3766,12 +3769,12 @@
       <c r="J66" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="P66" s="3"/>
+      <c r="P66" s="19"/>
       <c r="Q66" s="18"/>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="6">
         <v>19</v>
       </c>
@@ -3794,12 +3797,12 @@
       <c r="J67" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="P67" s="3"/>
+      <c r="P67" s="19"/>
       <c r="Q67" s="18"/>
     </row>
     <row r="68" spans="1:17" ht="33" x14ac:dyDescent="0.3">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
       <c r="C68" s="6">
         <v>20</v>
       </c>
@@ -3822,52 +3825,52 @@
       <c r="J68" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="P68" s="3"/>
+      <c r="P68" s="19"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P69" s="3"/>
+      <c r="P69" s="19"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P70" s="3"/>
+      <c r="P70" s="19"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P71" s="3"/>
+      <c r="P71" s="19"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P72" s="3"/>
+      <c r="P72" s="19"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P73" s="3"/>
+      <c r="P73" s="19"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P74" s="3"/>
+      <c r="P74" s="19"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P75" s="3"/>
+      <c r="P75" s="19"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P76" s="3"/>
+      <c r="P76" s="19"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P77" s="3"/>
+      <c r="P77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P78" s="3"/>
+      <c r="P78" s="19"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P79" s="3"/>
+      <c r="P79" s="19"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="P80" s="3"/>
+      <c r="P80" s="19"/>
     </row>
     <row r="81" spans="16:16" x14ac:dyDescent="0.3">
-      <c r="P81" s="3"/>
+      <c r="P81" s="19"/>
     </row>
     <row r="82" spans="16:16" x14ac:dyDescent="0.3">
-      <c r="P82" s="3"/>
+      <c r="P82" s="19"/>
     </row>
     <row r="83" spans="16:16" x14ac:dyDescent="0.3">
-      <c r="P83" s="3"/>
+      <c r="P83" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>